<commit_message>
Renamed from disposible to disposable
</commit_message>
<xml_diff>
--- a/Description of data/growth_disposable_income.xlsx
+++ b/Description of data/growth_disposable_income.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nielseriksen/applied_finance/Description of data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F34DA93D-FBE2-A14B-93D0-FDDD7326EB97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0C08EF-7E75-6141-B060-18339464A5FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23100" yWindow="7540" windowWidth="37220" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:AD16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>